<commit_message>
feat(shifts): process shifts from excel to solver data
</commit_message>
<xml_diff>
--- a/shiny/www/dataTemplate.xlsx
+++ b/shiny/www/dataTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samue\Desktop\tfm-repo\shiny\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73BA71CF-1C29-41FD-9870-3C6F0D61A5EC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE990D4-FF64-4547-9D0A-9E1F1EEEDDA4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{6639CBF0-1A6E-437C-903B-D5B18B74404F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="144">
   <si>
     <t>TW-01</t>
   </si>
@@ -441,6 +441,30 @@
   </si>
   <si>
     <t>T50</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>07:00 - 18:00; 19:00 - 06:00</t>
   </si>
 </sst>
 </file>
@@ -490,12 +514,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1019,64 +1044,176 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF9ABDA-8F5D-4FAD-87D9-353996B99213}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="13.1328125" customWidth="1"/>
     <col min="2" max="2" width="21.1328125" customWidth="1"/>
+    <col min="3" max="9" width="24.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>71</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C2" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>72</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C3" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>73</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C4" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>74</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C5" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>75</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(shifts): add push mode
</commit_message>
<xml_diff>
--- a/shiny/www/dataTemplate.xlsx
+++ b/shiny/www/dataTemplate.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samue\Desktop\tfm-repo\shiny\www\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samue\Documents\code\tfm-repo\shiny\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE990D4-FF64-4547-9D0A-9E1F1EEEDDA4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC15F051-A84B-4AFD-9301-D4A524622258}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{6639CBF0-1A6E-437C-903B-D5B18B74404F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{6639CBF0-1A6E-437C-903B-D5B18B74404F}"/>
   </bookViews>
   <sheets>
     <sheet name="jobs" sheetId="3" r:id="rId1"/>
     <sheet name="machines" sheetId="1" r:id="rId2"/>
     <sheet name="tasks" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -464,7 +463,7 @@
     <t>Sunday</t>
   </si>
   <si>
-    <t>07:00 - 18:00; 19:00 - 06:00</t>
+    <t>07:00 - 12:00; 13:00 - 18:00; 19:00 - 01:00</t>
   </si>
 </sst>
 </file>
@@ -841,15 +840,15 @@
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.796875" customWidth="1"/>
-    <col min="3" max="3" width="15.796875" customWidth="1"/>
+    <col min="2" max="2" width="23.77734375" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -866,7 +865,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>76</v>
       </c>
@@ -883,7 +882,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -900,7 +899,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>78</v>
       </c>
@@ -917,7 +916,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>79</v>
       </c>
@@ -934,7 +933,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>80</v>
       </c>
@@ -951,7 +950,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>81</v>
       </c>
@@ -968,7 +967,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>82</v>
       </c>
@@ -985,7 +984,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>83</v>
       </c>
@@ -1002,7 +1001,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>84</v>
       </c>
@@ -1019,7 +1018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>85</v>
       </c>
@@ -1046,18 +1045,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF9ABDA-8F5D-4FAD-87D9-353996B99213}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.1328125" customWidth="1"/>
-    <col min="2" max="2" width="21.1328125" customWidth="1"/>
-    <col min="3" max="9" width="24.265625" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" customWidth="1"/>
+    <col min="3" max="9" width="24.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1086,7 +1085,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>71</v>
       </c>
@@ -1112,7 +1111,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>72</v>
       </c>
@@ -1138,7 +1137,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -1164,7 +1163,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>74</v>
       </c>
@@ -1190,7 +1189,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>75</v>
       </c>
@@ -1226,20 +1225,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D94EBF3-B95F-4317-AA04-8FAA7B9C9F8E}">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47:C51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.46484375" customWidth="1"/>
-    <col min="4" max="4" width="12.796875" customWidth="1"/>
-    <col min="5" max="5" width="10.86328125" customWidth="1"/>
-    <col min="6" max="6" width="12.53125" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1259,7 +1258,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -1267,7 +1266,7 @@
         <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2">
         <v>21</v>
@@ -1276,7 +1275,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -1284,7 +1283,7 @@
         <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3">
         <v>34</v>
@@ -1296,7 +1295,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -1304,7 +1303,7 @@
         <v>76</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D4">
         <v>53</v>
@@ -1316,7 +1315,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>89</v>
       </c>
@@ -1336,7 +1335,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>90</v>
       </c>
@@ -1356,7 +1355,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>91</v>
       </c>
@@ -1364,7 +1363,7 @@
         <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D7">
         <v>16</v>
@@ -1373,7 +1372,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>92</v>
       </c>
@@ -1381,7 +1380,7 @@
         <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D8">
         <v>21</v>
@@ -1393,7 +1392,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>93</v>
       </c>
@@ -1413,7 +1412,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>94</v>
       </c>
@@ -1433,7 +1432,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>95</v>
       </c>
@@ -1441,7 +1440,7 @@
         <v>77</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D11">
         <v>71</v>
@@ -1453,7 +1452,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>96</v>
       </c>
@@ -1470,7 +1469,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>97</v>
       </c>
@@ -1478,7 +1477,7 @@
         <v>78</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13">
         <v>31</v>
@@ -1490,7 +1489,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>98</v>
       </c>
@@ -1498,7 +1497,7 @@
         <v>78</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D14">
         <v>39</v>
@@ -1510,7 +1509,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>99</v>
       </c>
@@ -1518,7 +1517,7 @@
         <v>78</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D15">
         <v>42</v>
@@ -1530,7 +1529,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>100</v>
       </c>
@@ -1550,7 +1549,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>101</v>
       </c>
@@ -1567,7 +1566,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>102</v>
       </c>
@@ -1575,7 +1574,7 @@
         <v>79</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D18">
         <v>66</v>
@@ -1587,7 +1586,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>103</v>
       </c>
@@ -1595,7 +1594,7 @@
         <v>79</v>
       </c>
       <c r="C19" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D19">
         <v>77</v>
@@ -1607,7 +1606,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>104</v>
       </c>
@@ -1627,7 +1626,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>105</v>
       </c>
@@ -1647,7 +1646,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>106</v>
       </c>
@@ -1655,7 +1654,7 @@
         <v>80</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D22">
         <v>19</v>
@@ -1664,7 +1663,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>107</v>
       </c>
@@ -1672,7 +1671,7 @@
         <v>80</v>
       </c>
       <c r="C23" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D23">
         <v>34</v>
@@ -1684,7 +1683,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>108</v>
       </c>
@@ -1692,7 +1691,7 @@
         <v>80</v>
       </c>
       <c r="C24" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D24">
         <v>37</v>
@@ -1704,7 +1703,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>109</v>
       </c>
@@ -1712,7 +1711,7 @@
         <v>80</v>
       </c>
       <c r="C25" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D25">
         <v>64</v>
@@ -1724,7 +1723,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>110</v>
       </c>
@@ -1732,7 +1731,7 @@
         <v>80</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D26">
         <v>83</v>
@@ -1744,7 +1743,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>111</v>
       </c>
@@ -1752,7 +1751,7 @@
         <v>81</v>
       </c>
       <c r="C27" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D27">
         <v>43</v>
@@ -1761,7 +1760,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>112</v>
       </c>
@@ -1781,7 +1780,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>113</v>
       </c>
@@ -1789,7 +1788,7 @@
         <v>81</v>
       </c>
       <c r="C29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D29">
         <v>62</v>
@@ -1801,7 +1800,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>114</v>
       </c>
@@ -1809,7 +1808,7 @@
         <v>81</v>
       </c>
       <c r="C30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D30">
         <v>79</v>
@@ -1821,7 +1820,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>115</v>
       </c>
@@ -1829,7 +1828,7 @@
         <v>81</v>
       </c>
       <c r="C31" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D31">
         <v>92</v>
@@ -1841,7 +1840,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>116</v>
       </c>
@@ -1849,7 +1848,7 @@
         <v>82</v>
       </c>
       <c r="C32" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D32">
         <v>69</v>
@@ -1858,7 +1857,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>117</v>
       </c>
@@ -1866,7 +1865,7 @@
         <v>82</v>
       </c>
       <c r="C33" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D33">
         <v>77</v>
@@ -1878,7 +1877,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>118</v>
       </c>
@@ -1886,7 +1885,7 @@
         <v>82</v>
       </c>
       <c r="C34" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D34">
         <v>87</v>
@@ -1898,7 +1897,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>119</v>
       </c>
@@ -1906,7 +1905,7 @@
         <v>82</v>
       </c>
       <c r="C35" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D35">
         <v>87</v>
@@ -1918,7 +1917,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>120</v>
       </c>
@@ -1926,7 +1925,7 @@
         <v>82</v>
       </c>
       <c r="C36" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D36">
         <v>93</v>
@@ -1938,7 +1937,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>121</v>
       </c>
@@ -1946,7 +1945,7 @@
         <v>83</v>
       </c>
       <c r="C37" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D37">
         <v>24</v>
@@ -1955,7 +1954,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>122</v>
       </c>
@@ -1963,7 +1962,7 @@
         <v>83</v>
       </c>
       <c r="C38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D38">
         <v>38</v>
@@ -1975,7 +1974,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>123</v>
       </c>
@@ -1983,7 +1982,7 @@
         <v>83</v>
       </c>
       <c r="C39" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D39">
         <v>41</v>
@@ -1995,7 +1994,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>124</v>
       </c>
@@ -2003,7 +2002,7 @@
         <v>83</v>
       </c>
       <c r="C40" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D40">
         <v>60</v>
@@ -2015,7 +2014,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>125</v>
       </c>
@@ -2035,7 +2034,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>126</v>
       </c>
@@ -2043,7 +2042,7 @@
         <v>84</v>
       </c>
       <c r="C42" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D42">
         <v>17</v>
@@ -2052,7 +2051,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>127</v>
       </c>
@@ -2060,7 +2059,7 @@
         <v>84</v>
       </c>
       <c r="C43" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D43">
         <v>25</v>
@@ -2072,7 +2071,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>128</v>
       </c>
@@ -2080,7 +2079,7 @@
         <v>84</v>
       </c>
       <c r="C44" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D44">
         <v>44</v>
@@ -2092,7 +2091,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>129</v>
       </c>
@@ -2100,7 +2099,7 @@
         <v>84</v>
       </c>
       <c r="C45" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D45">
         <v>49</v>
@@ -2112,7 +2111,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>130</v>
       </c>
@@ -2120,7 +2119,7 @@
         <v>84</v>
       </c>
       <c r="C46" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D46">
         <v>98</v>
@@ -2132,7 +2131,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>131</v>
       </c>
@@ -2140,7 +2139,7 @@
         <v>85</v>
       </c>
       <c r="C47" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D47">
         <v>43</v>
@@ -2149,7 +2148,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>132</v>
       </c>
@@ -2169,7 +2168,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>133</v>
       </c>
@@ -2177,7 +2176,7 @@
         <v>85</v>
       </c>
       <c r="C49" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D49">
         <v>96</v>
@@ -2189,7 +2188,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>134</v>
       </c>
@@ -2209,7 +2208,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>135</v>
       </c>
@@ -2217,7 +2216,7 @@
         <v>85</v>
       </c>
       <c r="C51" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D51">
         <v>96</v>
@@ -2230,7 +2229,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F51">
+  <sortState ref="A2:F51">
     <sortCondition ref="A1"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
feat(due dates): now due dates are input as datetimes
For now, if a solution is found for which no jobs are late, the objective value for that solution would be the makespan. But this is not accurate, as new solutions with little tardiness can be seen as improvements, but arent. To be fix in the future.
</commit_message>
<xml_diff>
--- a/shiny/www/dataTemplate.xlsx
+++ b/shiny/www/dataTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samue\Documents\code\tfm-repo\shiny\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC15F051-A84B-4AFD-9301-D4A524622258}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E426D9-998B-4504-8D7B-2C1862A46D1C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{6639CBF0-1A6E-437C-903B-D5B18B74404F}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="143">
   <si>
     <t>TW-01</t>
   </si>
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t>Machine Name</t>
-  </si>
-  <si>
-    <t>Job Release Date</t>
   </si>
   <si>
     <t>Job Due Date</t>
@@ -513,13 +510,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -834,23 +832,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94B56C77-D033-44C5-8405-8BE16B8FF683}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="23.77734375" customWidth="1"/>
-    <col min="3" max="3" width="15.77734375" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>5</v>
@@ -859,185 +856,153 @@
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4">
+        <v>43739.75</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>76</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>335</v>
-      </c>
-      <c r="E2">
+      <c r="C3" s="4">
+        <v>43740.75</v>
+      </c>
+      <c r="D3">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>77</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>242</v>
-      </c>
-      <c r="E3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="C4" s="4">
+        <v>43740.75</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>78</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>289</v>
-      </c>
-      <c r="E4">
+      <c r="C5" s="4">
+        <v>43740.75</v>
+      </c>
+      <c r="D5">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>79</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>460</v>
-      </c>
-      <c r="E5">
+      <c r="C6" s="4">
+        <v>43739.75</v>
+      </c>
+      <c r="D6">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>80</v>
       </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>308</v>
-      </c>
-      <c r="E6">
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="4">
+        <v>43742.75</v>
+      </c>
+      <c r="D7">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>81</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>429</v>
-      </c>
-      <c r="E7">
+      <c r="C8" s="4">
+        <v>43741.75</v>
+      </c>
+      <c r="D8">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>82</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>537</v>
-      </c>
-      <c r="E8">
+      <c r="C9" s="4">
+        <v>43740.75</v>
+      </c>
+      <c r="D9">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>83</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>320</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="C10" s="4">
+        <v>43739.75</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>84</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>17</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>303</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>85</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
+      <c r="C11" s="4">
+        <v>43739.75</v>
       </c>
       <c r="D11">
-        <v>506</v>
-      </c>
-      <c r="E11">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1053,7 +1018,8 @@
   <cols>
     <col min="1" max="1" width="13.109375" customWidth="1"/>
     <col min="2" max="2" width="21.109375" customWidth="1"/>
-    <col min="3" max="9" width="24.21875" customWidth="1"/>
+    <col min="3" max="3" width="46.109375" customWidth="1"/>
+    <col min="4" max="9" width="24.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -1064,155 +1030,155 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1225,7 +1191,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D94EBF3-B95F-4317-AA04-8FAA7B9C9F8E}">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C47" sqref="C47:C51"/>
     </sheetView>
   </sheetViews>
@@ -1240,992 +1206,992 @@
   <sheetData>
     <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2">
         <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3">
         <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4">
         <v>53</v>
       </c>
       <c r="E4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5">
         <v>55</v>
       </c>
       <c r="E5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6">
         <v>95</v>
       </c>
       <c r="E6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7">
         <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8">
         <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9">
         <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10">
         <v>52</v>
       </c>
       <c r="E10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11">
         <v>71</v>
       </c>
       <c r="E11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12">
         <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13">
         <v>31</v>
       </c>
       <c r="E13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14">
         <v>39</v>
       </c>
       <c r="E14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D15">
         <v>42</v>
       </c>
       <c r="E15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16">
         <v>98</v>
       </c>
       <c r="E16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17">
         <v>55</v>
       </c>
       <c r="E17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D18">
         <v>66</v>
       </c>
       <c r="E18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D19">
         <v>77</v>
       </c>
       <c r="E19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D20">
         <v>77</v>
       </c>
       <c r="E20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D21">
         <v>79</v>
       </c>
       <c r="E21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D22">
         <v>19</v>
       </c>
       <c r="E22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23">
         <v>34</v>
       </c>
       <c r="E23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D24">
         <v>37</v>
       </c>
       <c r="E24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D25">
         <v>64</v>
       </c>
       <c r="E25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D26">
         <v>83</v>
       </c>
       <c r="E26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F26" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D27">
         <v>43</v>
       </c>
       <c r="E27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D28">
         <v>54</v>
       </c>
       <c r="E28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D29">
         <v>62</v>
       </c>
       <c r="E29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D30">
         <v>79</v>
       </c>
       <c r="E30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D31">
         <v>92</v>
       </c>
       <c r="E31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D32">
         <v>69</v>
       </c>
       <c r="E32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D33">
         <v>77</v>
       </c>
       <c r="E33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F33" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D34">
         <v>87</v>
       </c>
       <c r="E34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F34" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B35" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D35">
         <v>87</v>
       </c>
       <c r="E35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D36">
         <v>93</v>
       </c>
       <c r="E36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F36" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B37" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D37">
         <v>24</v>
       </c>
       <c r="E37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B38" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D38">
         <v>38</v>
       </c>
       <c r="E38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F38" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B39" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D39">
         <v>41</v>
       </c>
       <c r="E39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F39" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B40" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C40" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D40">
         <v>60</v>
       </c>
       <c r="E40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F40" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C41" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D41">
         <v>83</v>
       </c>
       <c r="E41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F41" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B42" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C42" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D42">
         <v>17</v>
       </c>
       <c r="E42" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B43" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C43" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D43">
         <v>25</v>
       </c>
       <c r="E43" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F43" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B44" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D44">
         <v>44</v>
       </c>
       <c r="E44" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F44" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C45" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D45">
         <v>49</v>
       </c>
       <c r="E45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F45" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B46" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C46" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D46">
         <v>98</v>
       </c>
       <c r="E46" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F46" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B47" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C47" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D47">
         <v>43</v>
       </c>
       <c r="E47" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B48" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D48">
         <v>75</v>
       </c>
       <c r="E48" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F48" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B49" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C49" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D49">
         <v>96</v>
       </c>
       <c r="E49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F49" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B50" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C50" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D50">
         <v>79</v>
       </c>
       <c r="E50" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F50" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B51" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C51" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D51">
         <v>96</v>
       </c>
       <c r="E51" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F51" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(shifts): push mode corrected
</commit_message>
<xml_diff>
--- a/shiny/www/dataTemplate.xlsx
+++ b/shiny/www/dataTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samue\Documents\code\tfm-repo\shiny\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E426D9-998B-4504-8D7B-2C1862A46D1C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC04F97A-C357-4645-8744-847736E28050}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{6639CBF0-1A6E-437C-903B-D5B18B74404F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6639CBF0-1A6E-437C-903B-D5B18B74404F}"/>
   </bookViews>
   <sheets>
     <sheet name="jobs" sheetId="3" r:id="rId1"/>
@@ -834,8 +834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94B56C77-D033-44C5-8405-8BE16B8FF683}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -867,7 +867,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="4">
-        <v>43739.75</v>
+        <v>43746.75</v>
       </c>
       <c r="D2">
         <v>4</v>
@@ -881,7 +881,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="4">
-        <v>43740.75</v>
+        <v>43747.75</v>
       </c>
       <c r="D3">
         <v>4</v>
@@ -895,7 +895,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="4">
-        <v>43740.75</v>
+        <v>43745.75</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -909,7 +909,7 @@
         <v>16</v>
       </c>
       <c r="C5" s="4">
-        <v>43740.75</v>
+        <v>43746.75</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -923,7 +923,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="4">
-        <v>43739.75</v>
+        <v>43745.75</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -937,7 +937,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="4">
-        <v>43742.75</v>
+        <v>43746.75</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -951,7 +951,7 @@
         <v>14</v>
       </c>
       <c r="C8" s="4">
-        <v>43741.75</v>
+        <v>43746.75</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -965,7 +965,7 @@
         <v>15</v>
       </c>
       <c r="C9" s="4">
-        <v>43740.75</v>
+        <v>43745.75</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -979,7 +979,7 @@
         <v>16</v>
       </c>
       <c r="C10" s="4">
-        <v>43739.75</v>
+        <v>43745.75</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -993,7 +993,7 @@
         <v>17</v>
       </c>
       <c r="C11" s="4">
-        <v>43739.75</v>
+        <v>43745.75</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1010,7 +1010,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF9ABDA-8F5D-4FAD-87D9-353996B99213}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
doc: how it works
</commit_message>
<xml_diff>
--- a/shiny/www/dataTemplate.xlsx
+++ b/shiny/www/dataTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samue\Documents\code\tfm-repo\shiny\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC04F97A-C357-4645-8744-847736E28050}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF155705-32CD-4AD3-B265-C2BAEFA2A697}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6639CBF0-1A6E-437C-903B-D5B18B74404F}"/>
+    <workbookView xWindow="1404" yWindow="1416" windowWidth="19188" windowHeight="10260" xr2:uid="{6639CBF0-1A6E-437C-903B-D5B18B74404F}"/>
   </bookViews>
   <sheets>
     <sheet name="jobs" sheetId="3" r:id="rId1"/>
@@ -835,7 +835,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -867,7 +867,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="4">
-        <v>43746.75</v>
+        <v>43773.75</v>
       </c>
       <c r="D2">
         <v>4</v>
@@ -881,7 +881,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="4">
-        <v>43747.75</v>
+        <v>43773.75</v>
       </c>
       <c r="D3">
         <v>4</v>
@@ -895,7 +895,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="4">
-        <v>43745.75</v>
+        <v>43773.75</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -909,7 +909,7 @@
         <v>16</v>
       </c>
       <c r="C5" s="4">
-        <v>43746.75</v>
+        <v>43774.75</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -923,7 +923,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="4">
-        <v>43745.75</v>
+        <v>43775.75</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -937,7 +937,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="4">
-        <v>43746.75</v>
+        <v>43773.75</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -951,7 +951,7 @@
         <v>14</v>
       </c>
       <c r="C8" s="4">
-        <v>43746.75</v>
+        <v>43774.75</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -965,7 +965,7 @@
         <v>15</v>
       </c>
       <c r="C9" s="4">
-        <v>43745.75</v>
+        <v>43773.75</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -979,7 +979,7 @@
         <v>16</v>
       </c>
       <c r="C10" s="4">
-        <v>43745.75</v>
+        <v>43774.75</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -993,7 +993,7 @@
         <v>17</v>
       </c>
       <c r="C11" s="4">
-        <v>43745.75</v>
+        <v>43775.75</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1011,7 +1011,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1192,7 +1192,7 @@
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C47" sqref="C47:C51"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1201,7 +1201,7 @@
     <col min="3" max="3" width="14.44140625" customWidth="1"/>
     <col min="4" max="4" width="12.77734375" customWidth="1"/>
     <col min="5" max="5" width="10.88671875" customWidth="1"/>
-    <col min="6" max="6" width="12.5546875" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -1894,7 +1894,7 @@
         <v>53</v>
       </c>
       <c r="D36">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="E36" t="s">
         <v>70</v>
@@ -2195,7 +2195,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:F51">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F51">
     <sortCondition ref="A1"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>